<commit_message>
update result 20201120 & update plan 20201123
</commit_message>
<xml_diff>
--- a/20201120.xlsx
+++ b/20201120.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swan3\Desktop\plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BAC848C-DB1E-4446-B2A1-B1DDA9E08B81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C961E44-FBA2-4705-A541-9AAA0C3555EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-120" windowWidth="23256" windowHeight="12576" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
   <si>
     <t>일</t>
   </si>
@@ -138,10 +138,6 @@
   </si>
   <si>
     <t>할 일</t>
-    <phoneticPr fontId="21" type="noConversion"/>
-  </si>
-  <si>
-    <t>사유</t>
     <phoneticPr fontId="21" type="noConversion"/>
   </si>
   <si>
@@ -206,6 +202,26 @@
   </si>
   <si>
     <t>모빌리티 테스트 &amp; cp stat 9 전송</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>전날술먹음</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>늦게잠</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>일했음</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>안하고잤다</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>초과근무, 술</t>
     <phoneticPr fontId="21" type="noConversion"/>
   </si>
 </sst>
@@ -379,7 +395,7 @@
       <charset val="129"/>
     </font>
   </fonts>
-  <fills count="37">
+  <fills count="41">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -596,8 +612,32 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -727,6 +767,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -862,7 +939,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -896,49 +973,64 @@
     <xf numFmtId="176" fontId="1" fillId="32" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="176" fontId="1" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="37" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="37" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="37" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="38" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="39" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="39" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="37" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="38" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="38" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="36" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="38" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="40" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="40" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1474,24 +1566,24 @@
   <dimension ref="B2:M24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E3" sqref="E3:E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="16.5" customWidth="1"/>
-    <col min="3" max="3" width="48.8984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.09765625" customWidth="1"/>
-    <col min="5" max="5" width="85.69921875" customWidth="1"/>
-    <col min="6" max="6" width="16.3984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.19921875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.8984375" customWidth="1"/>
-    <col min="9" max="9" width="39.69921875" customWidth="1"/>
-    <col min="11" max="11" width="9.8984375" customWidth="1"/>
+    <col min="3" max="3" width="48.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.125" customWidth="1"/>
+    <col min="5" max="5" width="85.75" customWidth="1"/>
+    <col min="6" max="6" width="16.375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.875" customWidth="1"/>
+    <col min="9" max="9" width="39.75" customWidth="1"/>
+    <col min="11" max="11" width="9.875" customWidth="1"/>
     <col min="12" max="12" width="78" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1499,7 +1591,7 @@
         <v>0</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>30</v>
@@ -1527,18 +1619,20 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="2:13" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="C3" s="13" t="s">
+    <row r="3" spans="2:13" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" s="10"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="28" t="s">
         <v>45</v>
-      </c>
-      <c r="D3" s="14"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="23" t="s">
-        <v>46</v>
       </c>
       <c r="H3" s="8"/>
       <c r="I3" t="s">
@@ -1551,13 +1645,13 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.4">
-      <c r="B4" s="15"/>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B4" s="12"/>
       <c r="C4" s="16"/>
       <c r="D4" s="17"/>
       <c r="E4" s="10"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="23"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="28"/>
       <c r="H4" s="8"/>
       <c r="I4" t="s">
         <v>11</v>
@@ -1566,13 +1660,13 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.4">
-      <c r="B5" s="15"/>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B5" s="12"/>
       <c r="C5" s="16"/>
       <c r="D5" s="17"/>
       <c r="E5" s="10"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="23"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="28"/>
       <c r="H5" s="8"/>
       <c r="I5" t="s">
         <v>12</v>
@@ -1581,13 +1675,13 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.4">
-      <c r="B6" s="15"/>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B6" s="12"/>
       <c r="C6" s="16"/>
       <c r="D6" s="17"/>
       <c r="E6" s="10"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="23"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="28"/>
       <c r="H6" s="8"/>
       <c r="I6" t="s">
         <v>10</v>
@@ -1596,13 +1690,13 @@
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.4">
-      <c r="B7" s="15"/>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B7" s="12"/>
       <c r="C7" s="16"/>
       <c r="D7" s="17"/>
       <c r="E7" s="10"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="23"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="28"/>
       <c r="H7" s="8"/>
       <c r="I7" t="s">
         <v>8</v>
@@ -1615,13 +1709,13 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.4">
-      <c r="B8" s="15"/>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B8" s="12"/>
       <c r="C8" s="16"/>
       <c r="D8" s="17"/>
       <c r="E8" s="10"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="23"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="28"/>
       <c r="H8" s="8"/>
       <c r="I8" t="s">
         <v>4</v>
@@ -1630,206 +1724,214 @@
         <v>103</v>
       </c>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B9" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" s="10"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="8"/>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B10" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="18"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="8"/>
-    </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.4">
-      <c r="B10" s="9" t="s">
+      <c r="D10" s="20"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="8"/>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B11" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="D10" s="21"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="8"/>
-    </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.4">
-      <c r="B11" s="3" t="s">
+      <c r="C11" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" s="20"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="8"/>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B12" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="D11" s="18"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="8"/>
-    </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.4">
-      <c r="B12" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="21"/>
+      <c r="D12" s="20"/>
       <c r="E12" s="10"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="23"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="28"/>
       <c r="H12" s="8"/>
     </row>
-    <row r="13" spans="2:13" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="2:13" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D13" s="18"/>
+      <c r="C13" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" s="20"/>
       <c r="E13" s="10"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="23"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="28"/>
       <c r="H13" s="8"/>
     </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.4">
+    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B14" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D14" s="21"/>
+      <c r="D14" s="20"/>
       <c r="E14" s="10"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="23"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="28"/>
       <c r="H14" s="8"/>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D15" s="18"/>
+      <c r="C15" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" s="20"/>
       <c r="E15" s="10"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="24"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="29" t="s">
+        <v>52</v>
+      </c>
       <c r="H15" s="8"/>
     </row>
-    <row r="16" spans="2:13" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:13" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="21"/>
+      <c r="D16" s="20"/>
       <c r="E16" s="10"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="25"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="30"/>
       <c r="H16" s="8"/>
     </row>
-    <row r="17" spans="2:8" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:8" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D17" s="18"/>
+      <c r="C17" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="20"/>
       <c r="E17" s="10"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="25"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="30"/>
       <c r="H17" s="8"/>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B18" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="D18" s="21"/>
+      <c r="C18" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" s="20"/>
       <c r="E18" s="10"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="25"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="30"/>
       <c r="H18" s="8"/>
     </row>
-    <row r="19" spans="2:8" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:8" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D19" s="18"/>
+      <c r="C19" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" s="20"/>
       <c r="E19" s="10"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="25"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="30"/>
       <c r="H19" s="8"/>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B20" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="D20" s="22"/>
+      <c r="C20" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20" s="25" t="s">
+        <v>50</v>
+      </c>
       <c r="E20" s="10"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="25"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="30"/>
       <c r="H20" s="8"/>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B21" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D21" s="18"/>
+      <c r="C21" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="D21" s="26"/>
       <c r="E21" s="10"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="25"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="30"/>
       <c r="H21" s="8"/>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B22" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C22" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="D22" s="27"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="30"/>
+      <c r="H22" s="8"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B23" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="D22" s="21"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="25"/>
-      <c r="H22" s="8"/>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B23" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D23" s="20"/>
+      <c r="D23" s="24" t="s">
+        <v>51</v>
+      </c>
       <c r="E23" s="10"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="25"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="30"/>
       <c r="H23" s="8"/>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B24" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
     <mergeCell ref="G3:G14"/>
     <mergeCell ref="G15:G23"/>
     <mergeCell ref="E3:E23"/>
@@ -1838,6 +1940,7 @@
     <mergeCell ref="D3:D8"/>
     <mergeCell ref="F3:F14"/>
     <mergeCell ref="F15:F23"/>
+    <mergeCell ref="D20:D22"/>
   </mergeCells>
   <phoneticPr fontId="21" type="noConversion"/>
   <pageMargins left="0.69986110925674438" right="0.69986110925674438" top="0.75" bottom="0.75" header="0.30000001192092896" footer="0.30000001192092896"/>
@@ -1852,7 +1955,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <phoneticPr fontId="21" type="noConversion"/>
   <pageMargins left="0.69986110925674438" right="0.69986110925674438" top="0.75" bottom="0.75" header="0.30000001192092896" footer="0.30000001192092896"/>
@@ -1867,7 +1970,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <phoneticPr fontId="21" type="noConversion"/>
   <pageMargins left="0.69986110925674438" right="0.69986110925674438" top="0.75" bottom="0.75" header="0.30000001192092896" footer="0.30000001192092896"/>

</xml_diff>